<commit_message>
LJ 200 epochs 99% training data
</commit_message>
<xml_diff>
--- a/Base Model (LJ Speech)/LJ Experiments.xlsx
+++ b/Base Model (LJ Speech)/LJ Experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhvan\Documents\GitHub\P4P-Transformer-ASR-for-Dysarthric-Speech\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhvan\Documents\GitHub\P4P-Transformer-ASR-for-Dysarthric-Speech\Base Model (LJ Speech)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0642B2A3-3F06-4294-BC67-09CA15F01E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E726EF-CD47-4E6F-BDB3-2490BA8B4F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="15390" windowHeight="9442" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="100 epoches" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,14 @@
     <sheet name="200 epoches" sheetId="11" r:id="rId10"/>
     <sheet name="40 epoches with seed" sheetId="12" r:id="rId11"/>
     <sheet name="40+200+L3" sheetId="13" r:id="rId12"/>
+    <sheet name="Final model" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="35">
   <si>
     <t>&lt;__main__.DisplayOutputs object at 0x7fe956d0d0a0&gt;</t>
   </si>
@@ -130,6 +131,12 @@
   </si>
   <si>
     <t>Learning rate/3</t>
+  </si>
+  <si>
+    <t>Model Name: LJ_200_2.0.h5</t>
+  </si>
+  <si>
+    <t>WER: 0.88</t>
   </si>
 </sst>
 </file>
@@ -3107,6 +3114,1007 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="24695072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Final model'!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WER</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Final model'!$P$2:$P$242</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="241"/>
+                <c:pt idx="0">
+                  <c:v>1.6013982518384611</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.459235323501356</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4824317852546511</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9437216451321619</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1078450052472779</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4920722459727029</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4654211237845729</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3112096253197549</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.212087069439163</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1891113841226471</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.258312785335705</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.361267885011249</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3362649276870719</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2055035567537571</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.129780523982139</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.121572145564744</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.124784740207293</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.105708389438413</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.016693971196474</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.0099159450953561</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.96243808355815441</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.97849268850113003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.057138341852998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.029026078021438</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.0571469675484171</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99359069518645504</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.0392048265545799</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.0149460505933949</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.97720295919817779</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.97649079990821064</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.98021728520361473</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.037501841190648</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.0343153420297651</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.0049848498412011</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.97888444089348436</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.96831440682326386</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.92910301193140676</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9158777611337906</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.87108913075247296</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.87018117995757305</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.88247781445541951</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.88971203855260828</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.87796643300006771</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.84538630445601937</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.86927354184856109</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.86782183010323422</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.8608510832416375</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.86974643606692326</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.85837176722350372</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.81044932244634316</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.83998313366718647</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.83641277570820705</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.85626436067299083</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.88075227561991942</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.86133889985728418</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.97285411165146807</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.88894364462266717</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.85335794962337841</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.83482091149217585</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.80067540513391489</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.83369223490623401</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.86967841074353125</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.87308677384996913</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.87003526688475141</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.87979365017046107</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.87061586944830505</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.81753593276513292</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.83066921714278885</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.83985397899048175</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.81711728583958998</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.8439570248442172</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.83267019269168818</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.84447498803836585</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.82836412012071958</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.797588953971616</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.84185174536746588</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.89322057501590102</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.85678287045762891</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.84597979515506483</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.8711899994884077</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.82887669969860267</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.87690087663881788</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.87995925023223809</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.86721905301235469</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.86109605193238303</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.85897282126069563</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.8451767866584402</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.79197991163056503</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.81139629285536663</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.80888039319556848</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.8538321999172156</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.83924653613975475</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.81109944232974507</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.85663164062946495</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.83395838162945124</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.82922603267663531</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.83126150476707694</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.83177851380148204</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.83473508456964707</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.8176614681480816</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.8558735748978229</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.84436452326625466</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.84179677851100987</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.84424119173667289</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.84104061627047233</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.84845692481824653</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.8512741336510804</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.84956334444029102</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.86570693628021456</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.8489705401280575</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.85037166248354645</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.84839257190063277</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.86395098917780011</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.85787139169195259</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.85650590037729524</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.85892122402423665</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.85316804521071288</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.84722370830802696</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.84601718159198935</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.84450619258100035</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.81781050284886003</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.84194805253498295</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.81497625175743582</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.82098984018440724</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.81804510376140993</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.80970423663487712</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.81565282891668944</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.80806262417125374</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.81545928095649745</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.82224721203960516</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.80344520807285957</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.82144258034572704</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.81889935967750649</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.80646908527354788</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.81870145725098564</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.80168024262465098</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.79799507275384041</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.80718916971967658</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.7964981321943998</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.81297557081857763</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.83448271290656195</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.82615321034858769</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.81393884093957336</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.8195493555203397</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.82587818294291726</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.81912151444693948</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.82219396283188795</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.82183520700438206</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.83170732775643719</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.82518601388428381</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.82334192047769039</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.82967617679847683</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.82153674648501629</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.82952151847472266</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.83659981739399247</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.83039615096942088</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.8303579513218462</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.8457935437310613</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.84655660539765565</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.84643039789701036</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.85999047960768471</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.85129533360785115</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.84426694532946289</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.85217894283033768</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.84988420227993988</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.84338494074999049</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.84889559857043084</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.84389123691197443</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.84654480172235136</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.84963544175604333</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.84870623517114896</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.84041877187700942</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.85031270078928078</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.83711402446560457</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.84980784106567098</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.84140894829177815</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.84392163801592412</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.84367215165201137</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.84524906206044337</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.84218793048368679</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.84208690718633195</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.83219395087793446</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.84302482064222817</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.83814925010769026</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.83629006988573829</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.84022929832744431</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.84793503723722752</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.86043045888186609</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.85429890927205521</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.85781847997912608</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.86427920675235292</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.8563093761602395</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.8613672749341712</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.86167566362922576</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.85730778852425849</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.85913428751096621</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.85358146026632264</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.84501812506271978</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.85924733448554347</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.86171015788211269</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.88722201717216975</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.89313283390877862</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.98144028884727719</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.94376878619936888</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.87817028859711044</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.90468547626612195</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.91188996893600238</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.94835947892560735</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.9126738524611846</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.93895393414865258</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.93530579027815886</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.95588875650976568</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.92359047274936434</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.90025955911701738</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.94573257482414685</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.8982695677886543</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.95860970567379589</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.96159240379649147</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>1.0282874626161389</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.96867243309429329</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.95264589856658355</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.9432046324906288</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.90055953948023537</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.91064839568904565</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.87050487016996758</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.89553918255397491</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.9214639896287895</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.93202729569651122</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.92432852486701877</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.90574990811923883</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.90371325214937581</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.94030444886047704</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.97518541067048947</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.93187159922881535</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.92866078399988516</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.90136079637910627</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.94510756839562227</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.9420011584360134</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.97115458295637425</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.95396517717186347</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.93991415266194833</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FC34-48CD-94AB-6CEE9CA50DC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1800086079"/>
+        <c:axId val="1800090239"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1800086079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1800090239"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1800090239"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1800086079"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8541,6 +9549,46 @@
 </file>
 
 <file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10449,6 +11497,522 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15547,6 +17111,97 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>402982</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142940</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECD5674A-DA55-4788-8A99-9820211BC82B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1934309" y="366347"/>
+          <a:ext cx="4271596" cy="3256882"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>622788</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>13187</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>36634</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>8791</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6EC6EED-7134-0071-6860-F4E2D7F5DEF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -17916,8 +19571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3BF714-311F-43D7-BD99-09F631D0D07E}">
   <dimension ref="D1:P242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M12" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22181,6 +23836,1964 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C87D77-8C3B-413F-9D06-9F09CCB221C2}">
+  <dimension ref="D1:P242"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1.6013982518384611</v>
+      </c>
+    </row>
+    <row r="3" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>3.459235323501356</v>
+      </c>
+    </row>
+    <row r="4" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>3.4824317852546511</v>
+      </c>
+    </row>
+    <row r="5" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>2.9437216451321619</v>
+      </c>
+    </row>
+    <row r="6" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>2.1078450052472779</v>
+      </c>
+    </row>
+    <row r="7" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>1.4920722459727029</v>
+      </c>
+    </row>
+    <row r="8" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O8">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>1.4654211237845729</v>
+      </c>
+    </row>
+    <row r="9" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O9">
+        <v>7</v>
+      </c>
+      <c r="P9">
+        <v>1.3112096253197549</v>
+      </c>
+    </row>
+    <row r="10" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O10">
+        <v>8</v>
+      </c>
+      <c r="P10">
+        <v>1.212087069439163</v>
+      </c>
+    </row>
+    <row r="11" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O11">
+        <v>9</v>
+      </c>
+      <c r="P11">
+        <v>1.1891113841226471</v>
+      </c>
+    </row>
+    <row r="12" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O12">
+        <v>10</v>
+      </c>
+      <c r="P12">
+        <v>1.258312785335705</v>
+      </c>
+    </row>
+    <row r="13" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O13">
+        <v>11</v>
+      </c>
+      <c r="P13">
+        <v>1.361267885011249</v>
+      </c>
+    </row>
+    <row r="14" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O14">
+        <v>12</v>
+      </c>
+      <c r="P14">
+        <v>1.3362649276870719</v>
+      </c>
+    </row>
+    <row r="15" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O15">
+        <v>13</v>
+      </c>
+      <c r="P15">
+        <v>1.2055035567537571</v>
+      </c>
+    </row>
+    <row r="16" spans="4:16" x14ac:dyDescent="0.45">
+      <c r="O16">
+        <v>14</v>
+      </c>
+      <c r="P16">
+        <v>1.129780523982139</v>
+      </c>
+    </row>
+    <row r="17" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O17">
+        <v>15</v>
+      </c>
+      <c r="P17">
+        <v>1.121572145564744</v>
+      </c>
+    </row>
+    <row r="18" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O18">
+        <v>16</v>
+      </c>
+      <c r="P18">
+        <v>1.124784740207293</v>
+      </c>
+    </row>
+    <row r="19" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O19">
+        <v>17</v>
+      </c>
+      <c r="P19">
+        <v>1.105708389438413</v>
+      </c>
+    </row>
+    <row r="20" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O20">
+        <v>18</v>
+      </c>
+      <c r="P20">
+        <v>1.016693971196474</v>
+      </c>
+    </row>
+    <row r="21" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O21">
+        <v>19</v>
+      </c>
+      <c r="P21">
+        <v>1.0099159450953561</v>
+      </c>
+    </row>
+    <row r="22" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O22">
+        <v>20</v>
+      </c>
+      <c r="P22">
+        <v>0.96243808355815441</v>
+      </c>
+    </row>
+    <row r="23" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O23">
+        <v>21</v>
+      </c>
+      <c r="P23">
+        <v>0.97849268850113003</v>
+      </c>
+    </row>
+    <row r="24" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O24">
+        <v>22</v>
+      </c>
+      <c r="P24">
+        <v>1.057138341852998</v>
+      </c>
+    </row>
+    <row r="25" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O25">
+        <v>23</v>
+      </c>
+      <c r="P25">
+        <v>1.029026078021438</v>
+      </c>
+    </row>
+    <row r="26" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O26">
+        <v>24</v>
+      </c>
+      <c r="P26">
+        <v>1.0571469675484171</v>
+      </c>
+    </row>
+    <row r="27" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O27">
+        <v>25</v>
+      </c>
+      <c r="P27">
+        <v>0.99359069518645504</v>
+      </c>
+    </row>
+    <row r="28" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O28">
+        <v>26</v>
+      </c>
+      <c r="P28">
+        <v>1.0392048265545799</v>
+      </c>
+    </row>
+    <row r="29" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O29">
+        <v>27</v>
+      </c>
+      <c r="P29">
+        <v>1.0149460505933949</v>
+      </c>
+    </row>
+    <row r="30" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O30">
+        <v>28</v>
+      </c>
+      <c r="P30">
+        <v>0.97720295919817779</v>
+      </c>
+    </row>
+    <row r="31" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O31">
+        <v>29</v>
+      </c>
+      <c r="P31">
+        <v>0.97649079990821064</v>
+      </c>
+    </row>
+    <row r="32" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O32">
+        <v>30</v>
+      </c>
+      <c r="P32">
+        <v>0.98021728520361473</v>
+      </c>
+    </row>
+    <row r="33" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O33">
+        <v>31</v>
+      </c>
+      <c r="P33">
+        <v>1.037501841190648</v>
+      </c>
+    </row>
+    <row r="34" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O34">
+        <v>32</v>
+      </c>
+      <c r="P34">
+        <v>1.0343153420297651</v>
+      </c>
+    </row>
+    <row r="35" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O35">
+        <v>33</v>
+      </c>
+      <c r="P35">
+        <v>1.0049848498412011</v>
+      </c>
+    </row>
+    <row r="36" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O36">
+        <v>34</v>
+      </c>
+      <c r="P36">
+        <v>0.97888444089348436</v>
+      </c>
+    </row>
+    <row r="37" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O37">
+        <v>35</v>
+      </c>
+      <c r="P37">
+        <v>0.96831440682326386</v>
+      </c>
+    </row>
+    <row r="38" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O38">
+        <v>36</v>
+      </c>
+      <c r="P38">
+        <v>0.92910301193140676</v>
+      </c>
+    </row>
+    <row r="39" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O39">
+        <v>37</v>
+      </c>
+      <c r="P39">
+        <v>0.9158777611337906</v>
+      </c>
+    </row>
+    <row r="40" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O40">
+        <v>38</v>
+      </c>
+      <c r="P40">
+        <v>0.87108913075247296</v>
+      </c>
+    </row>
+    <row r="41" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O41">
+        <v>39</v>
+      </c>
+      <c r="P41">
+        <v>0.87018117995757305</v>
+      </c>
+    </row>
+    <row r="42" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O42">
+        <v>40</v>
+      </c>
+      <c r="P42">
+        <v>0.88247781445541951</v>
+      </c>
+    </row>
+    <row r="43" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O43">
+        <v>41</v>
+      </c>
+      <c r="P43">
+        <v>0.88971203855260828</v>
+      </c>
+    </row>
+    <row r="44" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O44">
+        <v>42</v>
+      </c>
+      <c r="P44">
+        <v>0.87796643300006771</v>
+      </c>
+    </row>
+    <row r="45" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O45">
+        <v>43</v>
+      </c>
+      <c r="P45">
+        <v>0.84538630445601937</v>
+      </c>
+    </row>
+    <row r="46" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O46">
+        <v>44</v>
+      </c>
+      <c r="P46">
+        <v>0.86927354184856109</v>
+      </c>
+    </row>
+    <row r="47" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O47">
+        <v>45</v>
+      </c>
+      <c r="P47">
+        <v>0.86782183010323422</v>
+      </c>
+    </row>
+    <row r="48" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O48">
+        <v>46</v>
+      </c>
+      <c r="P48">
+        <v>0.8608510832416375</v>
+      </c>
+    </row>
+    <row r="49" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O49">
+        <v>47</v>
+      </c>
+      <c r="P49">
+        <v>0.86974643606692326</v>
+      </c>
+    </row>
+    <row r="50" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O50">
+        <v>48</v>
+      </c>
+      <c r="P50">
+        <v>0.85837176722350372</v>
+      </c>
+    </row>
+    <row r="51" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O51">
+        <v>49</v>
+      </c>
+      <c r="P51">
+        <v>0.81044932244634316</v>
+      </c>
+    </row>
+    <row r="52" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O52">
+        <v>50</v>
+      </c>
+      <c r="P52">
+        <v>0.83998313366718647</v>
+      </c>
+    </row>
+    <row r="53" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O53">
+        <v>51</v>
+      </c>
+      <c r="P53">
+        <v>0.83641277570820705</v>
+      </c>
+    </row>
+    <row r="54" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O54">
+        <v>52</v>
+      </c>
+      <c r="P54">
+        <v>0.85626436067299083</v>
+      </c>
+    </row>
+    <row r="55" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O55">
+        <v>53</v>
+      </c>
+      <c r="P55">
+        <v>0.88075227561991942</v>
+      </c>
+    </row>
+    <row r="56" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O56">
+        <v>54</v>
+      </c>
+      <c r="P56">
+        <v>0.86133889985728418</v>
+      </c>
+    </row>
+    <row r="57" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O57">
+        <v>55</v>
+      </c>
+      <c r="P57">
+        <v>0.97285411165146807</v>
+      </c>
+    </row>
+    <row r="58" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O58">
+        <v>56</v>
+      </c>
+      <c r="P58">
+        <v>0.88894364462266717</v>
+      </c>
+    </row>
+    <row r="59" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O59">
+        <v>57</v>
+      </c>
+      <c r="P59">
+        <v>0.85335794962337841</v>
+      </c>
+    </row>
+    <row r="60" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O60">
+        <v>58</v>
+      </c>
+      <c r="P60">
+        <v>0.83482091149217585</v>
+      </c>
+    </row>
+    <row r="61" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O61">
+        <v>59</v>
+      </c>
+      <c r="P61">
+        <v>0.80067540513391489</v>
+      </c>
+    </row>
+    <row r="62" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O62">
+        <v>60</v>
+      </c>
+      <c r="P62">
+        <v>0.83369223490623401</v>
+      </c>
+    </row>
+    <row r="63" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O63">
+        <v>61</v>
+      </c>
+      <c r="P63">
+        <v>0.86967841074353125</v>
+      </c>
+    </row>
+    <row r="64" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O64">
+        <v>62</v>
+      </c>
+      <c r="P64">
+        <v>0.87308677384996913</v>
+      </c>
+    </row>
+    <row r="65" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O65">
+        <v>63</v>
+      </c>
+      <c r="P65">
+        <v>0.87003526688475141</v>
+      </c>
+    </row>
+    <row r="66" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O66">
+        <v>64</v>
+      </c>
+      <c r="P66">
+        <v>0.87979365017046107</v>
+      </c>
+    </row>
+    <row r="67" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O67">
+        <v>65</v>
+      </c>
+      <c r="P67">
+        <v>0.87061586944830505</v>
+      </c>
+    </row>
+    <row r="68" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O68">
+        <v>66</v>
+      </c>
+      <c r="P68">
+        <v>0.81753593276513292</v>
+      </c>
+    </row>
+    <row r="69" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O69">
+        <v>67</v>
+      </c>
+      <c r="P69">
+        <v>0.83066921714278885</v>
+      </c>
+    </row>
+    <row r="70" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O70">
+        <v>68</v>
+      </c>
+      <c r="P70">
+        <v>0.83985397899048175</v>
+      </c>
+    </row>
+    <row r="71" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O71">
+        <v>69</v>
+      </c>
+      <c r="P71">
+        <v>0.81711728583958998</v>
+      </c>
+    </row>
+    <row r="72" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O72">
+        <v>70</v>
+      </c>
+      <c r="P72">
+        <v>0.8439570248442172</v>
+      </c>
+    </row>
+    <row r="73" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O73">
+        <v>71</v>
+      </c>
+      <c r="P73">
+        <v>0.83267019269168818</v>
+      </c>
+    </row>
+    <row r="74" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O74">
+        <v>72</v>
+      </c>
+      <c r="P74">
+        <v>0.84447498803836585</v>
+      </c>
+    </row>
+    <row r="75" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O75">
+        <v>73</v>
+      </c>
+      <c r="P75">
+        <v>0.82836412012071958</v>
+      </c>
+    </row>
+    <row r="76" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O76">
+        <v>74</v>
+      </c>
+      <c r="P76">
+        <v>0.797588953971616</v>
+      </c>
+    </row>
+    <row r="77" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O77">
+        <v>75</v>
+      </c>
+      <c r="P77">
+        <v>0.84185174536746588</v>
+      </c>
+    </row>
+    <row r="78" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O78">
+        <v>76</v>
+      </c>
+      <c r="P78">
+        <v>0.89322057501590102</v>
+      </c>
+    </row>
+    <row r="79" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O79">
+        <v>77</v>
+      </c>
+      <c r="P79">
+        <v>0.85678287045762891</v>
+      </c>
+    </row>
+    <row r="80" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O80">
+        <v>78</v>
+      </c>
+      <c r="P80">
+        <v>0.84597979515506483</v>
+      </c>
+    </row>
+    <row r="81" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O81">
+        <v>79</v>
+      </c>
+      <c r="P81">
+        <v>0.8711899994884077</v>
+      </c>
+    </row>
+    <row r="82" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O82">
+        <v>80</v>
+      </c>
+      <c r="P82">
+        <v>0.82887669969860267</v>
+      </c>
+    </row>
+    <row r="83" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O83">
+        <v>81</v>
+      </c>
+      <c r="P83">
+        <v>0.87690087663881788</v>
+      </c>
+    </row>
+    <row r="84" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O84">
+        <v>82</v>
+      </c>
+      <c r="P84">
+        <v>0.87995925023223809</v>
+      </c>
+    </row>
+    <row r="85" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O85">
+        <v>83</v>
+      </c>
+      <c r="P85">
+        <v>0.86721905301235469</v>
+      </c>
+    </row>
+    <row r="86" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O86">
+        <v>84</v>
+      </c>
+      <c r="P86">
+        <v>0.86109605193238303</v>
+      </c>
+    </row>
+    <row r="87" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O87">
+        <v>85</v>
+      </c>
+      <c r="P87">
+        <v>0.85897282126069563</v>
+      </c>
+    </row>
+    <row r="88" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O88">
+        <v>86</v>
+      </c>
+      <c r="P88">
+        <v>0.8451767866584402</v>
+      </c>
+    </row>
+    <row r="89" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O89">
+        <v>87</v>
+      </c>
+      <c r="P89">
+        <v>0.79197991163056503</v>
+      </c>
+    </row>
+    <row r="90" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O90">
+        <v>88</v>
+      </c>
+      <c r="P90">
+        <v>0.81139629285536663</v>
+      </c>
+    </row>
+    <row r="91" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O91">
+        <v>89</v>
+      </c>
+      <c r="P91">
+        <v>0.80888039319556848</v>
+      </c>
+    </row>
+    <row r="92" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O92">
+        <v>90</v>
+      </c>
+      <c r="P92">
+        <v>0.8538321999172156</v>
+      </c>
+    </row>
+    <row r="93" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O93">
+        <v>91</v>
+      </c>
+      <c r="P93">
+        <v>0.83924653613975475</v>
+      </c>
+    </row>
+    <row r="94" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O94">
+        <v>92</v>
+      </c>
+      <c r="P94">
+        <v>0.81109944232974507</v>
+      </c>
+    </row>
+    <row r="95" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O95">
+        <v>93</v>
+      </c>
+      <c r="P95">
+        <v>0.85663164062946495</v>
+      </c>
+    </row>
+    <row r="96" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O96">
+        <v>94</v>
+      </c>
+      <c r="P96">
+        <v>0.83395838162945124</v>
+      </c>
+    </row>
+    <row r="97" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O97">
+        <v>95</v>
+      </c>
+      <c r="P97">
+        <v>0.82922603267663531</v>
+      </c>
+    </row>
+    <row r="98" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O98">
+        <v>96</v>
+      </c>
+      <c r="P98">
+        <v>0.83126150476707694</v>
+      </c>
+    </row>
+    <row r="99" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O99">
+        <v>97</v>
+      </c>
+      <c r="P99">
+        <v>0.83177851380148204</v>
+      </c>
+    </row>
+    <row r="100" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O100">
+        <v>98</v>
+      </c>
+      <c r="P100">
+        <v>0.83473508456964707</v>
+      </c>
+    </row>
+    <row r="101" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O101">
+        <v>99</v>
+      </c>
+      <c r="P101">
+        <v>0.8176614681480816</v>
+      </c>
+    </row>
+    <row r="102" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O102">
+        <v>100</v>
+      </c>
+      <c r="P102">
+        <v>0.8558735748978229</v>
+      </c>
+    </row>
+    <row r="103" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O103">
+        <v>101</v>
+      </c>
+      <c r="P103">
+        <v>0.84436452326625466</v>
+      </c>
+    </row>
+    <row r="104" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O104">
+        <v>102</v>
+      </c>
+      <c r="P104">
+        <v>0.84179677851100987</v>
+      </c>
+    </row>
+    <row r="105" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O105">
+        <v>103</v>
+      </c>
+      <c r="P105">
+        <v>0.84424119173667289</v>
+      </c>
+    </row>
+    <row r="106" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O106">
+        <v>104</v>
+      </c>
+      <c r="P106">
+        <v>0.84104061627047233</v>
+      </c>
+    </row>
+    <row r="107" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O107">
+        <v>105</v>
+      </c>
+      <c r="P107">
+        <v>0.84845692481824653</v>
+      </c>
+    </row>
+    <row r="108" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O108">
+        <v>106</v>
+      </c>
+      <c r="P108">
+        <v>0.8512741336510804</v>
+      </c>
+    </row>
+    <row r="109" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O109">
+        <v>107</v>
+      </c>
+      <c r="P109">
+        <v>0.84956334444029102</v>
+      </c>
+    </row>
+    <row r="110" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O110">
+        <v>108</v>
+      </c>
+      <c r="P110">
+        <v>0.86570693628021456</v>
+      </c>
+    </row>
+    <row r="111" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O111">
+        <v>109</v>
+      </c>
+      <c r="P111">
+        <v>0.8489705401280575</v>
+      </c>
+    </row>
+    <row r="112" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O112">
+        <v>110</v>
+      </c>
+      <c r="P112">
+        <v>0.85037166248354645</v>
+      </c>
+    </row>
+    <row r="113" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O113">
+        <v>111</v>
+      </c>
+      <c r="P113">
+        <v>0.84839257190063277</v>
+      </c>
+    </row>
+    <row r="114" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O114">
+        <v>112</v>
+      </c>
+      <c r="P114">
+        <v>0.86395098917780011</v>
+      </c>
+    </row>
+    <row r="115" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O115">
+        <v>113</v>
+      </c>
+      <c r="P115">
+        <v>0.85787139169195259</v>
+      </c>
+    </row>
+    <row r="116" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O116">
+        <v>114</v>
+      </c>
+      <c r="P116">
+        <v>0.85650590037729524</v>
+      </c>
+    </row>
+    <row r="117" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O117">
+        <v>115</v>
+      </c>
+      <c r="P117">
+        <v>0.85892122402423665</v>
+      </c>
+    </row>
+    <row r="118" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O118">
+        <v>116</v>
+      </c>
+      <c r="P118">
+        <v>0.85316804521071288</v>
+      </c>
+    </row>
+    <row r="119" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O119">
+        <v>117</v>
+      </c>
+      <c r="P119">
+        <v>0.84722370830802696</v>
+      </c>
+    </row>
+    <row r="120" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O120">
+        <v>118</v>
+      </c>
+      <c r="P120">
+        <v>0.84601718159198935</v>
+      </c>
+    </row>
+    <row r="121" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O121">
+        <v>119</v>
+      </c>
+      <c r="P121">
+        <v>0.84450619258100035</v>
+      </c>
+    </row>
+    <row r="122" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O122">
+        <v>120</v>
+      </c>
+      <c r="P122">
+        <v>0.81781050284886003</v>
+      </c>
+    </row>
+    <row r="123" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O123">
+        <v>121</v>
+      </c>
+      <c r="P123">
+        <v>0.84194805253498295</v>
+      </c>
+    </row>
+    <row r="124" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O124">
+        <v>122</v>
+      </c>
+      <c r="P124">
+        <v>0.81497625175743582</v>
+      </c>
+    </row>
+    <row r="125" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O125">
+        <v>123</v>
+      </c>
+      <c r="P125">
+        <v>0.82098984018440724</v>
+      </c>
+    </row>
+    <row r="126" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O126">
+        <v>124</v>
+      </c>
+      <c r="P126">
+        <v>0.81804510376140993</v>
+      </c>
+    </row>
+    <row r="127" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O127">
+        <v>125</v>
+      </c>
+      <c r="P127">
+        <v>0.80970423663487712</v>
+      </c>
+    </row>
+    <row r="128" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O128">
+        <v>126</v>
+      </c>
+      <c r="P128">
+        <v>0.81565282891668944</v>
+      </c>
+    </row>
+    <row r="129" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O129">
+        <v>127</v>
+      </c>
+      <c r="P129">
+        <v>0.80806262417125374</v>
+      </c>
+    </row>
+    <row r="130" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O130">
+        <v>128</v>
+      </c>
+      <c r="P130">
+        <v>0.81545928095649745</v>
+      </c>
+    </row>
+    <row r="131" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O131">
+        <v>129</v>
+      </c>
+      <c r="P131">
+        <v>0.82224721203960516</v>
+      </c>
+    </row>
+    <row r="132" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O132">
+        <v>130</v>
+      </c>
+      <c r="P132">
+        <v>0.80344520807285957</v>
+      </c>
+    </row>
+    <row r="133" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O133">
+        <v>131</v>
+      </c>
+      <c r="P133">
+        <v>0.82144258034572704</v>
+      </c>
+    </row>
+    <row r="134" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O134">
+        <v>132</v>
+      </c>
+      <c r="P134">
+        <v>0.81889935967750649</v>
+      </c>
+    </row>
+    <row r="135" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O135">
+        <v>133</v>
+      </c>
+      <c r="P135">
+        <v>0.80646908527354788</v>
+      </c>
+    </row>
+    <row r="136" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O136">
+        <v>134</v>
+      </c>
+      <c r="P136">
+        <v>0.81870145725098564</v>
+      </c>
+    </row>
+    <row r="137" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O137">
+        <v>135</v>
+      </c>
+      <c r="P137">
+        <v>0.80168024262465098</v>
+      </c>
+    </row>
+    <row r="138" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O138">
+        <v>136</v>
+      </c>
+      <c r="P138">
+        <v>0.79799507275384041</v>
+      </c>
+    </row>
+    <row r="139" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O139">
+        <v>137</v>
+      </c>
+      <c r="P139">
+        <v>0.80718916971967658</v>
+      </c>
+    </row>
+    <row r="140" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O140">
+        <v>138</v>
+      </c>
+      <c r="P140">
+        <v>0.7964981321943998</v>
+      </c>
+    </row>
+    <row r="141" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O141">
+        <v>139</v>
+      </c>
+      <c r="P141">
+        <v>0.81297557081857763</v>
+      </c>
+    </row>
+    <row r="142" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O142">
+        <v>140</v>
+      </c>
+      <c r="P142">
+        <v>0.83448271290656195</v>
+      </c>
+    </row>
+    <row r="143" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O143">
+        <v>141</v>
+      </c>
+      <c r="P143">
+        <v>0.82615321034858769</v>
+      </c>
+    </row>
+    <row r="144" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O144">
+        <v>142</v>
+      </c>
+      <c r="P144">
+        <v>0.81393884093957336</v>
+      </c>
+    </row>
+    <row r="145" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O145">
+        <v>143</v>
+      </c>
+      <c r="P145">
+        <v>0.8195493555203397</v>
+      </c>
+    </row>
+    <row r="146" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O146">
+        <v>144</v>
+      </c>
+      <c r="P146">
+        <v>0.82587818294291726</v>
+      </c>
+    </row>
+    <row r="147" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O147">
+        <v>145</v>
+      </c>
+      <c r="P147">
+        <v>0.81912151444693948</v>
+      </c>
+    </row>
+    <row r="148" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O148">
+        <v>146</v>
+      </c>
+      <c r="P148">
+        <v>0.82219396283188795</v>
+      </c>
+    </row>
+    <row r="149" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O149">
+        <v>147</v>
+      </c>
+      <c r="P149">
+        <v>0.82183520700438206</v>
+      </c>
+    </row>
+    <row r="150" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O150">
+        <v>148</v>
+      </c>
+      <c r="P150">
+        <v>0.83170732775643719</v>
+      </c>
+    </row>
+    <row r="151" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O151">
+        <v>149</v>
+      </c>
+      <c r="P151">
+        <v>0.82518601388428381</v>
+      </c>
+    </row>
+    <row r="152" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O152">
+        <v>150</v>
+      </c>
+      <c r="P152">
+        <v>0.82334192047769039</v>
+      </c>
+    </row>
+    <row r="153" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O153">
+        <v>151</v>
+      </c>
+      <c r="P153">
+        <v>0.82967617679847683</v>
+      </c>
+    </row>
+    <row r="154" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O154">
+        <v>152</v>
+      </c>
+      <c r="P154">
+        <v>0.82153674648501629</v>
+      </c>
+    </row>
+    <row r="155" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O155">
+        <v>153</v>
+      </c>
+      <c r="P155">
+        <v>0.82952151847472266</v>
+      </c>
+    </row>
+    <row r="156" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O156">
+        <v>154</v>
+      </c>
+      <c r="P156">
+        <v>0.83659981739399247</v>
+      </c>
+    </row>
+    <row r="157" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O157">
+        <v>155</v>
+      </c>
+      <c r="P157">
+        <v>0.83039615096942088</v>
+      </c>
+    </row>
+    <row r="158" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O158">
+        <v>156</v>
+      </c>
+      <c r="P158">
+        <v>0.8303579513218462</v>
+      </c>
+    </row>
+    <row r="159" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O159">
+        <v>157</v>
+      </c>
+      <c r="P159">
+        <v>0.8457935437310613</v>
+      </c>
+    </row>
+    <row r="160" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O160">
+        <v>158</v>
+      </c>
+      <c r="P160">
+        <v>0.84655660539765565</v>
+      </c>
+    </row>
+    <row r="161" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O161">
+        <v>159</v>
+      </c>
+      <c r="P161">
+        <v>0.84643039789701036</v>
+      </c>
+    </row>
+    <row r="162" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O162">
+        <v>160</v>
+      </c>
+      <c r="P162">
+        <v>0.85999047960768471</v>
+      </c>
+    </row>
+    <row r="163" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O163">
+        <v>161</v>
+      </c>
+      <c r="P163">
+        <v>0.85129533360785115</v>
+      </c>
+    </row>
+    <row r="164" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O164">
+        <v>162</v>
+      </c>
+      <c r="P164">
+        <v>0.84426694532946289</v>
+      </c>
+    </row>
+    <row r="165" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O165">
+        <v>163</v>
+      </c>
+      <c r="P165">
+        <v>0.85217894283033768</v>
+      </c>
+    </row>
+    <row r="166" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O166">
+        <v>164</v>
+      </c>
+      <c r="P166">
+        <v>0.84988420227993988</v>
+      </c>
+    </row>
+    <row r="167" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O167">
+        <v>165</v>
+      </c>
+      <c r="P167">
+        <v>0.84338494074999049</v>
+      </c>
+    </row>
+    <row r="168" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O168">
+        <v>166</v>
+      </c>
+      <c r="P168">
+        <v>0.84889559857043084</v>
+      </c>
+    </row>
+    <row r="169" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O169">
+        <v>167</v>
+      </c>
+      <c r="P169">
+        <v>0.84389123691197443</v>
+      </c>
+    </row>
+    <row r="170" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O170">
+        <v>168</v>
+      </c>
+      <c r="P170">
+        <v>0.84654480172235136</v>
+      </c>
+    </row>
+    <row r="171" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O171">
+        <v>169</v>
+      </c>
+      <c r="P171">
+        <v>0.84963544175604333</v>
+      </c>
+    </row>
+    <row r="172" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O172">
+        <v>170</v>
+      </c>
+      <c r="P172">
+        <v>0.84870623517114896</v>
+      </c>
+    </row>
+    <row r="173" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O173">
+        <v>171</v>
+      </c>
+      <c r="P173">
+        <v>0.84041877187700942</v>
+      </c>
+    </row>
+    <row r="174" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O174">
+        <v>172</v>
+      </c>
+      <c r="P174">
+        <v>0.85031270078928078</v>
+      </c>
+    </row>
+    <row r="175" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O175">
+        <v>173</v>
+      </c>
+      <c r="P175">
+        <v>0.83711402446560457</v>
+      </c>
+    </row>
+    <row r="176" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O176">
+        <v>174</v>
+      </c>
+      <c r="P176">
+        <v>0.84980784106567098</v>
+      </c>
+    </row>
+    <row r="177" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O177">
+        <v>175</v>
+      </c>
+      <c r="P177">
+        <v>0.84140894829177815</v>
+      </c>
+    </row>
+    <row r="178" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O178">
+        <v>176</v>
+      </c>
+      <c r="P178">
+        <v>0.84392163801592412</v>
+      </c>
+    </row>
+    <row r="179" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O179">
+        <v>177</v>
+      </c>
+      <c r="P179">
+        <v>0.84367215165201137</v>
+      </c>
+    </row>
+    <row r="180" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O180">
+        <v>178</v>
+      </c>
+      <c r="P180">
+        <v>0.84524906206044337</v>
+      </c>
+    </row>
+    <row r="181" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O181">
+        <v>179</v>
+      </c>
+      <c r="P181">
+        <v>0.84218793048368679</v>
+      </c>
+    </row>
+    <row r="182" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O182">
+        <v>180</v>
+      </c>
+      <c r="P182">
+        <v>0.84208690718633195</v>
+      </c>
+    </row>
+    <row r="183" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O183">
+        <v>181</v>
+      </c>
+      <c r="P183">
+        <v>0.83219395087793446</v>
+      </c>
+    </row>
+    <row r="184" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O184">
+        <v>182</v>
+      </c>
+      <c r="P184">
+        <v>0.84302482064222817</v>
+      </c>
+    </row>
+    <row r="185" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O185">
+        <v>183</v>
+      </c>
+      <c r="P185">
+        <v>0.83814925010769026</v>
+      </c>
+    </row>
+    <row r="186" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O186">
+        <v>184</v>
+      </c>
+      <c r="P186">
+        <v>0.83629006988573829</v>
+      </c>
+    </row>
+    <row r="187" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O187">
+        <v>185</v>
+      </c>
+      <c r="P187">
+        <v>0.84022929832744431</v>
+      </c>
+    </row>
+    <row r="188" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O188">
+        <v>186</v>
+      </c>
+      <c r="P188">
+        <v>0.84793503723722752</v>
+      </c>
+    </row>
+    <row r="189" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O189">
+        <v>187</v>
+      </c>
+      <c r="P189">
+        <v>0.86043045888186609</v>
+      </c>
+    </row>
+    <row r="190" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O190">
+        <v>188</v>
+      </c>
+      <c r="P190">
+        <v>0.85429890927205521</v>
+      </c>
+    </row>
+    <row r="191" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O191">
+        <v>189</v>
+      </c>
+      <c r="P191">
+        <v>0.85781847997912608</v>
+      </c>
+    </row>
+    <row r="192" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O192">
+        <v>190</v>
+      </c>
+      <c r="P192">
+        <v>0.86427920675235292</v>
+      </c>
+    </row>
+    <row r="193" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O193">
+        <v>191</v>
+      </c>
+      <c r="P193">
+        <v>0.8563093761602395</v>
+      </c>
+    </row>
+    <row r="194" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O194">
+        <v>192</v>
+      </c>
+      <c r="P194">
+        <v>0.8613672749341712</v>
+      </c>
+    </row>
+    <row r="195" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O195">
+        <v>193</v>
+      </c>
+      <c r="P195">
+        <v>0.86167566362922576</v>
+      </c>
+    </row>
+    <row r="196" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O196">
+        <v>194</v>
+      </c>
+      <c r="P196">
+        <v>0.85730778852425849</v>
+      </c>
+    </row>
+    <row r="197" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O197">
+        <v>195</v>
+      </c>
+      <c r="P197">
+        <v>0.85913428751096621</v>
+      </c>
+    </row>
+    <row r="198" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O198">
+        <v>196</v>
+      </c>
+      <c r="P198">
+        <v>0.85358146026632264</v>
+      </c>
+    </row>
+    <row r="199" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O199">
+        <v>197</v>
+      </c>
+      <c r="P199">
+        <v>0.84501812506271978</v>
+      </c>
+    </row>
+    <row r="200" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O200">
+        <v>198</v>
+      </c>
+      <c r="P200">
+        <v>0.85924733448554347</v>
+      </c>
+    </row>
+    <row r="201" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O201">
+        <v>199</v>
+      </c>
+      <c r="P201">
+        <v>0.86171015788211269</v>
+      </c>
+    </row>
+    <row r="202" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O202" t="s">
+        <v>23</v>
+      </c>
+      <c r="P202">
+        <v>0.88722201717216975</v>
+      </c>
+    </row>
+    <row r="203" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O203" t="s">
+        <v>23</v>
+      </c>
+      <c r="P203">
+        <v>0.89313283390877862</v>
+      </c>
+    </row>
+    <row r="204" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O204" t="s">
+        <v>23</v>
+      </c>
+      <c r="P204">
+        <v>0.98144028884727719</v>
+      </c>
+    </row>
+    <row r="205" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O205" t="s">
+        <v>23</v>
+      </c>
+      <c r="P205">
+        <v>0.94376878619936888</v>
+      </c>
+    </row>
+    <row r="206" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O206" t="s">
+        <v>23</v>
+      </c>
+      <c r="P206">
+        <v>0.87817028859711044</v>
+      </c>
+    </row>
+    <row r="207" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O207" t="s">
+        <v>23</v>
+      </c>
+      <c r="P207">
+        <v>0.90468547626612195</v>
+      </c>
+    </row>
+    <row r="208" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O208" t="s">
+        <v>23</v>
+      </c>
+      <c r="P208">
+        <v>0.91188996893600238</v>
+      </c>
+    </row>
+    <row r="209" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O209" t="s">
+        <v>23</v>
+      </c>
+      <c r="P209">
+        <v>0.94835947892560735</v>
+      </c>
+    </row>
+    <row r="210" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O210" t="s">
+        <v>23</v>
+      </c>
+      <c r="P210">
+        <v>0.9126738524611846</v>
+      </c>
+    </row>
+    <row r="211" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O211" t="s">
+        <v>23</v>
+      </c>
+      <c r="P211">
+        <v>0.93895393414865258</v>
+      </c>
+    </row>
+    <row r="212" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O212" t="s">
+        <v>23</v>
+      </c>
+      <c r="P212">
+        <v>0.93530579027815886</v>
+      </c>
+    </row>
+    <row r="213" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O213" t="s">
+        <v>23</v>
+      </c>
+      <c r="P213">
+        <v>0.95588875650976568</v>
+      </c>
+    </row>
+    <row r="214" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O214" t="s">
+        <v>23</v>
+      </c>
+      <c r="P214">
+        <v>0.92359047274936434</v>
+      </c>
+    </row>
+    <row r="215" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O215" t="s">
+        <v>23</v>
+      </c>
+      <c r="P215">
+        <v>0.90025955911701738</v>
+      </c>
+    </row>
+    <row r="216" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O216" t="s">
+        <v>23</v>
+      </c>
+      <c r="P216">
+        <v>0.94573257482414685</v>
+      </c>
+    </row>
+    <row r="217" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O217" t="s">
+        <v>23</v>
+      </c>
+      <c r="P217">
+        <v>0.8982695677886543</v>
+      </c>
+    </row>
+    <row r="218" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O218" t="s">
+        <v>23</v>
+      </c>
+      <c r="P218">
+        <v>0.95860970567379589</v>
+      </c>
+    </row>
+    <row r="219" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O219" t="s">
+        <v>23</v>
+      </c>
+      <c r="P219">
+        <v>0.96159240379649147</v>
+      </c>
+    </row>
+    <row r="220" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O220" t="s">
+        <v>23</v>
+      </c>
+      <c r="P220">
+        <v>1.0282874626161389</v>
+      </c>
+    </row>
+    <row r="221" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O221" t="s">
+        <v>23</v>
+      </c>
+      <c r="P221">
+        <v>0.96867243309429329</v>
+      </c>
+    </row>
+    <row r="222" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O222" t="s">
+        <v>23</v>
+      </c>
+      <c r="P222">
+        <v>0.95264589856658355</v>
+      </c>
+    </row>
+    <row r="223" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O223" t="s">
+        <v>23</v>
+      </c>
+      <c r="P223">
+        <v>0.9432046324906288</v>
+      </c>
+    </row>
+    <row r="224" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O224" t="s">
+        <v>23</v>
+      </c>
+      <c r="P224">
+        <v>0.90055953948023537</v>
+      </c>
+    </row>
+    <row r="225" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O225" t="s">
+        <v>23</v>
+      </c>
+      <c r="P225">
+        <v>0.91064839568904565</v>
+      </c>
+    </row>
+    <row r="226" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O226" t="s">
+        <v>23</v>
+      </c>
+      <c r="P226">
+        <v>0.87050487016996758</v>
+      </c>
+    </row>
+    <row r="227" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O227" t="s">
+        <v>23</v>
+      </c>
+      <c r="P227">
+        <v>0.89553918255397491</v>
+      </c>
+    </row>
+    <row r="228" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O228" t="s">
+        <v>23</v>
+      </c>
+      <c r="P228">
+        <v>0.9214639896287895</v>
+      </c>
+    </row>
+    <row r="229" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O229" t="s">
+        <v>23</v>
+      </c>
+      <c r="P229">
+        <v>0.93202729569651122</v>
+      </c>
+    </row>
+    <row r="230" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O230" t="s">
+        <v>23</v>
+      </c>
+      <c r="P230">
+        <v>0.92432852486701877</v>
+      </c>
+    </row>
+    <row r="231" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O231" t="s">
+        <v>23</v>
+      </c>
+      <c r="P231">
+        <v>0.90574990811923883</v>
+      </c>
+    </row>
+    <row r="232" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O232" t="s">
+        <v>23</v>
+      </c>
+      <c r="P232">
+        <v>0.90371325214937581</v>
+      </c>
+    </row>
+    <row r="233" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O233" t="s">
+        <v>23</v>
+      </c>
+      <c r="P233">
+        <v>0.94030444886047704</v>
+      </c>
+    </row>
+    <row r="234" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O234" t="s">
+        <v>23</v>
+      </c>
+      <c r="P234">
+        <v>0.97518541067048947</v>
+      </c>
+    </row>
+    <row r="235" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O235" t="s">
+        <v>23</v>
+      </c>
+      <c r="P235">
+        <v>0.93187159922881535</v>
+      </c>
+    </row>
+    <row r="236" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O236" t="s">
+        <v>23</v>
+      </c>
+      <c r="P236">
+        <v>0.92866078399988516</v>
+      </c>
+    </row>
+    <row r="237" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O237" t="s">
+        <v>23</v>
+      </c>
+      <c r="P237">
+        <v>0.90136079637910627</v>
+      </c>
+    </row>
+    <row r="238" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O238" t="s">
+        <v>23</v>
+      </c>
+      <c r="P238">
+        <v>0.94510756839562227</v>
+      </c>
+    </row>
+    <row r="239" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O239" t="s">
+        <v>23</v>
+      </c>
+      <c r="P239">
+        <v>0.9420011584360134</v>
+      </c>
+    </row>
+    <row r="240" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O240" t="s">
+        <v>23</v>
+      </c>
+      <c r="P240">
+        <v>0.97115458295637425</v>
+      </c>
+    </row>
+    <row r="241" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O241" t="s">
+        <v>23</v>
+      </c>
+      <c r="P241">
+        <v>0.95396517717186347</v>
+      </c>
+    </row>
+    <row r="242" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O242" t="s">
+        <v>23</v>
+      </c>
+      <c r="P242">
+        <v>0.93991415266194833</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A72DB2-0D67-4A3C-977B-3CC349AC5AD0}">
   <dimension ref="A1:D41"/>

</xml_diff>